<commit_message>
Import Export - User & Level
</commit_message>
<xml_diff>
--- a/public/template_level.xlsx
+++ b/public/template_level.xlsx
@@ -27,12 +27,15 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
     <t>level_kode</t>
   </si>
   <si>
     <t>level_nama</t>
+  </si>
+  <si>
+    <t>KRU</t>
   </si>
   <si>
     <t>Kurir</t>
@@ -659,11 +662,8 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1">
@@ -1202,13 +1202,13 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelRow="1" outlineLevelCol="3"/>
+  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelRow="1" outlineLevelCol="1"/>
   <cols>
     <col min="1" max="1" width="14.2857142857143" customWidth="1"/>
     <col min="2" max="2" width="14.4285714285714" customWidth="1"/>
@@ -1216,22 +1216,20 @@
     <col min="4" max="4" width="17.5714285714286" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" s="1" customFormat="1" spans="1:4">
-      <c r="A1" s="2" t="s">
+    <row r="1" s="1" customFormat="1" spans="1:2">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2"/>
-      <c r="D1" s="2"/>
     </row>
     <row r="2" spans="1:2">
-      <c r="A2">
-        <v>5</v>
+      <c r="A2" t="s">
+        <v>2</v>
       </c>
       <c r="B2" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>